<commit_message>
part c almost done
</commit_message>
<xml_diff>
--- a/Lab 3 Data.xlsx
+++ b/Lab 3 Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/jessijha_upenn_edu/Documents/Spring 2024/ESE 3500/Lab 3 - Theremin/lab-3-theremin-jsjha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{D6A24699-E61E-4639-988C-DF2BBD90B850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{527AF2E6-B707-4A96-B1FE-7382E840A610}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{D6A24699-E61E-4639-988C-DF2BBD90B850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD6C6D5C-E645-4FEF-B9ED-C7A8B9B3112F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8E5CACB6-192B-4FA3-9921-A1B2A9816AB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8E5CACB6-192B-4FA3-9921-A1B2A9816AB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part A" sheetId="1" r:id="rId1"/>
+    <sheet name="Part C" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -376,6 +377,133 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97EAAF70-1BB9-4765-8416-9CC77038D4B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1143000"/>
+          <a:ext cx="9753600" cy="7896225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C88F7EF2-9440-412D-9391-2A93E5A0DB7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10582275" y="1143000"/>
+          <a:ext cx="9753600" cy="7896225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -682,7 +810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E196B0A0-0B9F-407B-9A51-DD9876A1A371}">
   <dimension ref="D1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -702,4 +830,28 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8803BA18-1297-4B64-AC9E-2E67EB02A45A}">
+  <dimension ref="E50:S50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="O55" sqref="O55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="50" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="S50">
+        <v>56.79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>